<commit_message>
add pynum and pandas test program
</commit_message>
<xml_diff>
--- a/pynum/test.xlsx
+++ b/pynum/test.xlsx
@@ -411,16 +411,16 @@
         <v>42602</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6351224701321139</v>
+        <v>0.3830520358464513</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8563754812735298</v>
+        <v>0.8947454165326297</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2045067698099069</v>
+        <v>0.6327228580167067</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5404261885992665</v>
+        <v>0.4240862509183345</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -428,16 +428,16 @@
         <v>42603</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5100874611936471</v>
+        <v>0.7596543070440361</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5437310844479901</v>
+        <v>0.6465080687461903</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7980857289840904</v>
+        <v>0.59483642934008</v>
       </c>
       <c r="E3" t="n">
-        <v>0.09051198079081235</v>
+        <v>0.2693498587946093</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -445,16 +445,16 @@
         <v>42604</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1635798255180422</v>
+        <v>0.4369891931017392</v>
       </c>
       <c r="C4" t="n">
-        <v>0.752640154970505</v>
+        <v>0.2750477894891764</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8655251845937489</v>
+        <v>0.5590702820641964</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1066308137261054</v>
+        <v>0.2384682983040076</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -462,16 +462,16 @@
         <v>42605</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3434682271256014</v>
+        <v>0.761972593927858</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5204086779128538</v>
+        <v>0.9404414338443914</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4187482555952511</v>
+        <v>0.1252523231592332</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05270694658652009</v>
+        <v>0.6136490322132813</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -479,16 +479,16 @@
         <v>42606</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6668149294927741</v>
+        <v>0.2120530015793479</v>
       </c>
       <c r="C6" t="n">
-        <v>0.737530524461136</v>
+        <v>0.945671954701841</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5919105696369171</v>
+        <v>0.6392771840427417</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3334580311094052</v>
+        <v>0.8740041794208206</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -496,16 +496,16 @@
         <v>42607</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6676659502303031</v>
+        <v>0.9141177053444617</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7595262551985483</v>
+        <v>0.8362416142071636</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6606048677456933</v>
+        <v>0.2074197608251617</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4934600525651606</v>
+        <v>0.2823075770737018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>